<commit_message>
Changes for mandatory attribute
</commit_message>
<xml_diff>
--- a/src/assets/images/Sample Mapping File.xlsx
+++ b/src/assets/images/Sample Mapping File.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Courses\AngularJS\Angular WS\ETL\src\assets\images\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data Migration Project\Persistent Microservices\src\assets\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC8B71D7-75F9-4D3A-BD6A-D4902B767476}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{859D5484-A755-49BD-A239-8B8951CA5E53}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>destination_value</t>
   </si>
@@ -34,6 +34,15 @@
   </si>
   <si>
     <t>admin_type</t>
+  </si>
+  <si>
+    <t>is_Mandatory</t>
+  </si>
+  <si>
+    <t>default_value</t>
+  </si>
+  <si>
+    <t>enable_check_for_invalid</t>
   </si>
 </sst>
 </file>
@@ -351,15 +360,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -368,6 +377,15 @@
       </c>
       <c r="C1" t="s">
         <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>